<commit_message>
"break" to "brake" across all documents and scripts
</commit_message>
<xml_diff>
--- a/key_arduinopins.xlsx
+++ b/key_arduinopins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stuberadmin\Documents\GitHub\headfixed_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956BFD04-19B4-4699-A88F-B13B90F3C1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321162AC-BB7D-4E74-A9D7-1377A9F8D6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9710" yWindow="760" windowWidth="26490" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,12 +81,6 @@
     <t>start; break</t>
   </si>
   <si>
-    <t>0;18</t>
-  </si>
-  <si>
-    <t>servo 3 (radial)</t>
-  </si>
-  <si>
     <t>bnc ttl 1</t>
   </si>
   <si>
@@ -202,6 +196,12 @@
   </si>
   <si>
     <t>TTL Back Block 12</t>
+  </si>
+  <si>
+    <t>servo 3 (brake)</t>
+  </si>
+  <si>
+    <t>0; 20</t>
   </si>
 </sst>
 </file>
@@ -575,7 +575,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -712,7 +712,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -720,7 +720,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="C9" s="2">
         <v>11</v>
@@ -729,10 +729,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -740,13 +740,13 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -754,13 +754,13 @@
         <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="2">
         <v>3</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
@@ -768,13 +768,13 @@
         <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3">
         <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -782,13 +782,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="2">
         <v>21</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -796,13 +796,13 @@
         <v>6</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1">
         <v>22</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -810,13 +810,13 @@
         <v>6</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="1">
         <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -824,13 +824,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1">
         <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -838,13 +838,13 @@
         <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2">
         <v>25</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -852,7 +852,7 @@
         <v>6</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C18" s="4">
         <v>12</v>
@@ -866,13 +866,13 @@
         <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1">
         <v>26</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -880,13 +880,13 @@
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C20" s="1">
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -894,13 +894,13 @@
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1">
         <v>28</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -908,13 +908,13 @@
         <v>6</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C22" s="1">
         <v>29</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -922,13 +922,13 @@
         <v>6</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1">
         <v>30</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -936,13 +936,13 @@
         <v>6</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="1">
         <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -950,13 +950,13 @@
         <v>6</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1">
         <v>32</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -964,13 +964,13 @@
         <v>6</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1">
         <v>33</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -978,13 +978,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1">
         <v>34</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -992,13 +992,13 @@
         <v>6</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1">
         <v>35</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -1006,13 +1006,13 @@
         <v>6</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29" s="1">
         <v>36</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -1020,13 +1020,13 @@
         <v>6</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1">
         <v>37</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -1034,13 +1034,13 @@
         <v>6</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C31" s="1">
         <v>38</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -1048,13 +1048,13 @@
         <v>6</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C32" s="2">
         <v>39</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -1062,13 +1062,13 @@
         <v>6</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" s="1">
         <v>41</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -1076,13 +1076,13 @@
         <v>6</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" s="1">
         <v>42</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1090,13 +1090,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C35" s="1">
         <v>43</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1104,13 +1104,13 @@
         <v>6</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1">
         <v>44</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1118,13 +1118,13 @@
         <v>6</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C37" s="1">
         <v>45</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1132,13 +1132,13 @@
         <v>6</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="1">
         <v>46</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1146,13 +1146,13 @@
         <v>6</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39" s="1">
         <v>47</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1160,13 +1160,13 @@
         <v>6</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C40" s="1">
         <v>48</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1174,13 +1174,13 @@
         <v>6</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C41" s="1">
         <v>49</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1188,13 +1188,13 @@
         <v>6</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C42" s="1">
         <v>50</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1202,13 +1202,13 @@
         <v>6</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C43" s="1">
         <v>51</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1216,13 +1216,13 @@
         <v>6</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C44" s="1">
         <v>52</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>